<commit_message>
Add custom structure factor and 010 structure functions
</commit_message>
<xml_diff>
--- a/bt_test_data_calculations.xlsx
+++ b/bt_test_data_calculations.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommacgregor/Documents/GitHub/structure_factor_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{04B9CFA6-F3D8-D941-A372-2FF419311A0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFDF10-B232-4949-8E5D-27190954643A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="9000" windowWidth="28040" windowHeight="17440" xr2:uid="{67FA153E-4CB8-AD43-AAE3-F7D311E9A345}"/>
+    <workbookView xWindow="5560" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{67FA153E-4CB8-AD43-AAE3-F7D311E9A345}"/>
   </bookViews>
   <sheets>
     <sheet name="bt_test_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -641,7 +642,7 @@
         <v>2.695326600798964E-15</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I6" si="3">H3^2</f>
+        <f t="shared" ref="I3:I5" si="3">H3^2</f>
         <v>7.264785484974498E-30</v>
       </c>
       <c r="J3" t="str">

</xml_diff>